<commit_message>
Grant Type Profile Added
</commit_message>
<xml_diff>
--- a/src/main/java/TestSuite/MDOT/TestCases/MDOT/Recall_Confirm.xlsx
+++ b/src/main/java/TestSuite/MDOT/TestCases/MDOT/Recall_Confirm.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\athakur\Documents\MDOT\rstar\rstars\src\main\java\TestSuite\MDOT\TestCases\MDOT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pdighe\Documents\MDOT\Rstars-Automation\src\main\java\TestSuite\MDOT\TestCases\MDOT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F3D446-DCA9-4751-9BE6-5C911AB44036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706CB5D4-7A73-467E-B261-BCAD4881AFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -477,7 +477,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>